<commit_message>
extrapolation bug fix, added zero_age_depth
</commit_message>
<xml_diff>
--- a/input_highsierra/bd_highsierra.xlsx
+++ b/input_highsierra/bd_highsierra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrea/Documents/docs/src/Python/ESD_thermotrace/ESD_thermotrace_public/input_highsierra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDA2CBC-437D-9E45-98C7-F89051C08B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E7471B-8526-8744-9F6B-88BA55B435C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="11340" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>age</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>age_u</t>
+  </si>
+  <si>
+    <t>zero_age_depth</t>
   </si>
 </sst>
 </file>
@@ -876,15 +879,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -900,8 +906,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>-118.205833</v>
       </c>
@@ -918,7 +927,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>-118.20757999999999</v>
       </c>
@@ -935,7 +944,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>-118.216667</v>
       </c>
@@ -952,7 +961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>-118.21688</v>
       </c>
@@ -969,7 +978,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>-118.244722</v>
       </c>
@@ -986,7 +995,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>-118.22069</v>
       </c>
@@ -1003,7 +1012,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>-118.27555599999999</v>
       </c>
@@ -1020,7 +1029,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>-118.286389</v>
       </c>
@@ -1037,7 +1046,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>-118.291667</v>
       </c>

</xml_diff>